<commit_message>
POM integration and signup flow addition
</commit_message>
<xml_diff>
--- a/app/src/test/resources/testdata/testData.xlsx
+++ b/app/src/test/resources/testdata/testData.xlsx
@@ -4,7 +4,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="checkoutUsingExistingAccount" sheetId="1" r:id="rId1"/>
-    <sheet name="TestCase01" sheetId="2" r:id="rId2"/>
+    <sheet name="signUpWithPhoneNumber" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -444,13 +444,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>COUNTRY_CODE</v>
+      </c>
+      <c r="B1" t="str">
+        <v>OTP</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>IN</v>
+      </c>
+      <c r="B2" t="str">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>US</v>
+      </c>
+      <c r="B3" t="str">
+        <v>1111</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>